<commit_message>
Additinal codes are added in the description
The additional codes are in the yellow marked descriptions.
</commit_message>
<xml_diff>
--- a/Documents/RDBES Data Model CS.xlsx
+++ b/Documents/RDBES Data Model CS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icesit-my.sharepoint.com/personal/maria_makri_ices_dk/Documents/Profile/Desktop/Maria_ICES_dataflows/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icesit-my.sharepoint.com/personal/maria_makri_ices_dk/Documents/Profile/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="8_{879C7060-C235-4878-966B-C050AC75B5CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC66A3B3-4EE6-4806-9562-1D26A8BCCD05}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="8_{879C7060-C235-4878-966B-C050AC75B5CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CFDD7D45-7C25-4A7A-A851-54CA4C561147}"/>
   <bookViews>
-    <workbookView xWindow="28905" yWindow="60" windowWidth="21060" windowHeight="20745" tabRatio="781" firstSheet="7" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="781" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model v1.19.27" sheetId="1" r:id="rId1"/>
@@ -4679,9 +4679,6 @@
     <t>The source of the geographical data. The source of the geographical data. When GeographicalDataBasis is  “Official”, allowed codes are:  "Logb", "SalN", "PosDat", "VMS", "NotApplicable".  When GeographicalDataBasis is  “Estimated”, allowed codes are:"HarbLoc", "PosDat", "Crew", "Observer", "Exprt", "CombOD", "NotApplicable". When  GeographicalDataBasis is  “Measured”, allowed codes are: "Crew", "Observer", Report “Unknown” and “Not Applicable” when GeographicalDataBasis is “Unknown” and “Not Applicable” respectively.</t>
   </si>
   <si>
-    <t>Independent Duration recorded by independent staff deployed onboard (observers, control).  When DurationDataBasis is  “Estimated”, allowed codes are: "Exprt", "Crew", "Observer", "NotApplicable"  When DurationDataBasis is  “Measured”, allowed codes are:  "Crew" and "Observer". Report “Unknown” and “Not Applicable” when DataBasisOfStatisticalRectangle is “Unknown” and “Not Applicable” respectively.</t>
-  </si>
-  <si>
     <t>Total Weight measured. Data are determined from: “Official”, "Estimated" or "Measured" data.</t>
   </si>
   <si>
@@ -4689,6 +4686,9 @@
   </si>
   <si>
     <t>The source of the gear data.  When GearDataBasis is  “Official”, allowed codes are: "Logb" (Logbook), "CombOD" (Combination of official data sources), "ΟthDF" (Other declarative forms), "NotApplicable".  When GearDataBasis is  “Estimated”, allowed codes are:"SampDS" (Survey Data), "SampDC" )Commercial sampling data), "Exprt" (Expert Evaluation), "CombOD", "Crew", "Observer", "NotApplicable". When  GearDataBasis is  “Measured”, allowed codes are: "Crew", "Observer", Report “Unknown” and “Not Applicable” when GearDataBasis is “Unknown” and “Not Applicable” respectively.</t>
+  </si>
+  <si>
+    <t>Independent Duration recorded by independent staff deployed onboard (observers, control). When DurationDataBasis is  “Official”, allowed codes are "Logb" "CombOD" , "OthDF". When DurationDataBasis is  “Estimated”, allowed codes are: "Exprt", "Crew", "Observer", "NotApplicable"  When DurationDataBasis is  “Measured”, allowed codes are:  "Crew" and "Observer". Report “Unknown” and “Not Applicable” when DataBasisOfStatisticalRectangle is “Unknown” and “Not Applicable” respectively.</t>
   </si>
 </sst>
 </file>
@@ -6158,7 +6158,7 @@
         <v>The stratum of this record, 'U' if unstratified</v>
       </c>
     </row>
-    <row r="10" spans="1:35" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:35" ht="62" x14ac:dyDescent="0.35">
       <c r="A10" s="9">
         <f>IF(ISBLANK(Design!A10)=TRUE, Design!B10, "")</f>
         <v>0</v>
@@ -6890,7 +6890,7 @@
         <v>The method of selecting fish</v>
       </c>
     </row>
-    <row r="19" spans="9:35" ht="108.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="9:35" ht="93" x14ac:dyDescent="0.35">
       <c r="I19" s="9">
         <f>IF(ISBLANK('Temporal Event'!A9)=TRUE, 'Temporal Event'!B9, "")</f>
         <v>0</v>
@@ -8982,7 +8982,7 @@
         <v>Name or code of the cluster selected for sampling</v>
       </c>
     </row>
-    <row r="81" spans="9:15" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="81" spans="9:15" ht="31" x14ac:dyDescent="0.35">
       <c r="N81" s="10" t="str">
         <f>IF(ISBLANK('Landing event'!A18)=TRUE, 'Landing event'!F18, "")</f>
         <v>LEsampler</v>
@@ -10764,7 +10764,7 @@
         <v>1453</v>
       </c>
       <c r="L40" s="75" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="M40" s="71"/>
       <c r="N40" s="23"/>
@@ -28599,7 +28599,7 @@
       <c r="N15" s="32"/>
       <c r="O15" s="32"/>
     </row>
-    <row r="16" spans="1:15" ht="144" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" ht="156" x14ac:dyDescent="0.35">
       <c r="A16" s="52"/>
       <c r="B16" s="52"/>
       <c r="C16" s="52" t="s">
@@ -30357,7 +30357,7 @@
       <c r="U18" s="23"/>
       <c r="V18" s="23"/>
     </row>
-    <row r="19" spans="1:22" s="13" customFormat="1" ht="72" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:22" s="13" customFormat="1" ht="60" x14ac:dyDescent="0.35">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -30692,7 +30692,7 @@
         <v>1453</v>
       </c>
       <c r="L26" s="75" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
       <c r="M26" s="6"/>
       <c r="N26" s="23"/>
@@ -30705,7 +30705,7 @@
       <c r="U26" s="23"/>
       <c r="V26" s="23"/>
     </row>
-    <row r="27" spans="1:22" s="13" customFormat="1" ht="96.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:22" s="13" customFormat="1" ht="84.5" x14ac:dyDescent="0.35">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -30952,7 +30952,7 @@
         <v>1453</v>
       </c>
       <c r="L32" s="71" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="M32" s="6"/>
       <c r="N32" s="23"/>
@@ -31813,7 +31813,7 @@
         <v>1454</v>
       </c>
       <c r="L53" s="71" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="M53" s="6"/>
       <c r="N53" s="23"/>
@@ -31908,7 +31908,7 @@
       <c r="U55" s="23"/>
       <c r="V55" s="23"/>
     </row>
-    <row r="56" spans="1:22" ht="48.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:22" ht="36.5" x14ac:dyDescent="0.35">
       <c r="A56" s="5"/>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
@@ -32936,7 +32936,7 @@
   </sheetPr>
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
@@ -34321,7 +34321,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" ht="60.5" x14ac:dyDescent="0.35">
       <c r="A13" s="21"/>
       <c r="B13" s="21"/>
       <c r="C13" s="21"/>
@@ -34352,7 +34352,7 @@
         <v>1332</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="60.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" ht="48.5" x14ac:dyDescent="0.35">
       <c r="A14" s="21"/>
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
@@ -36301,7 +36301,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="48.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" ht="36.5" x14ac:dyDescent="0.35">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -37621,7 +37621,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="36.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" ht="24.5" x14ac:dyDescent="0.35">
       <c r="A21" s="21"/>
       <c r="B21" s="21"/>
       <c r="C21" s="21"/>
@@ -39097,7 +39097,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="36.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" ht="24.5" x14ac:dyDescent="0.35">
       <c r="A33" s="21"/>
       <c r="B33" s="21"/>
       <c r="C33" s="21"/>
@@ -39482,9 +39482,9 @@
   </sheetPr>
   <dimension ref="A1:N75"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K34" sqref="K34"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H42" sqref="A42:XFD42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -40176,7 +40176,7 @@
         <v>1498</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" ht="71.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -40205,7 +40205,7 @@
         <v>1453</v>
       </c>
       <c r="L21" s="75" t="s">
-        <v>1513</v>
+        <v>1516</v>
       </c>
       <c r="M21" s="21" t="s">
         <v>1509</v>
@@ -40648,7 +40648,7 @@
         <v>1453</v>
       </c>
       <c r="L34" s="75" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
       <c r="M34" s="71" t="s">
         <v>1511</v>
@@ -40890,7 +40890,7 @@
       </c>
       <c r="M41" s="71"/>
     </row>
-    <row r="42" spans="1:14" ht="111" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:14" ht="98" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
@@ -40919,7 +40919,7 @@
         <v>1453</v>
       </c>
       <c r="L42" s="71" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="M42" s="71"/>
     </row>
@@ -43057,15 +43057,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100584B29A9F606E64BBE0B94B46ABEDBD5" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ad12f995843361ff338b3798f1f5f41c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4d5313c0-c1e6-4122-afa9-da1ccdba405d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8fda66a02b6b5d1f39f2000ab0f58af4" ns2:_="">
     <xsd:import namespace="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
@@ -43237,6 +43228,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -43250,14 +43250,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04CD8B6C-25F0-471A-A724-387AC1B5060F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F67F35D-1CDD-4110-B6CE-1A6865489AEE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -43271,6 +43263,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04CD8B6C-25F0-471A-A724-387AC1B5060F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>